<commit_message>
Read VOL file header and SLO data. WARNING: Dates in header have note been parsed properly.
</commit_message>
<xml_diff>
--- a/inst/exdata/heyex_structure.xlsx
+++ b/inst/exdata/heyex_structure.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-24640" yWindow="0" windowWidth="24600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="header" sheetId="1" r:id="rId1"/>
-    <sheet name="bscan_header" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="header" sheetId="1" r:id="rId2"/>
+    <sheet name="bscan_header" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="127">
   <si>
     <t>Version</t>
   </si>
@@ -218,13 +219,196 @@
   </si>
   <si>
     <t xml:space="preserve">    header$spare            &lt;- readBin(vol_file, character(), size = 1840, endian = "little")</t>
+  </si>
+  <si>
+    <t>switch (readIntLittleEndian(raf)) {</t>
+  </si>
+  <si>
+    <t>String fileVersion=readByteString(raf, 12, 0);</t>
+  </si>
+  <si>
+    <t>byte(unicode Char), length=12, file offset=0, format of raw file version such as "HSF-OCT-101";</t>
+  </si>
+  <si>
+    <t>int sizeX=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=12, number of A-scans per B-scan, determines width, in pixels, of the oct image;</t>
+  </si>
+  <si>
+    <t>int numBscans=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=16, number of B-Scans in OCT file, determines the number of slices of an oct stack;</t>
+  </si>
+  <si>
+    <t>int sizeZ=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=20, number of samples per A-Scan, determines the height, in pixels, of the oct image;</t>
+  </si>
+  <si>
+    <t>double scaleX=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file offset=24, width of an A-Scan pixel in mm (optical resolution calculated using corneal curvature prior to export), determines pixel width of oct image;</t>
+  </si>
+  <si>
+    <t>double scaleY=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file offset=32, distance interval between B-Scans in mm, determines the pixel depth of an oct stack;</t>
+  </si>
+  <si>
+    <t>double scaleZ=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file offset=40, height of an A-scan pixel in mm (oct resolution between reflectance depths), determines the pixel height of oct image;</t>
+  </si>
+  <si>
+    <t>int sizeXSlo=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=48, width of SLO in pixels, determines width, in pixels, of the SLO image;</t>
+  </si>
+  <si>
+    <t>int sizeYSlo=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=52, height of SLO in pixels, determines height, in pixels, of the SLO image;</t>
+  </si>
+  <si>
+    <t>double scaleXSlo=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file offset=56, width of an SLO pixel in mm, determines pixel width of SLO image;</t>
+  </si>
+  <si>
+    <t>double scaleYSlo=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file offset=64, height of an SLO pixel in mm, determines pixel height of SLO image;</t>
+  </si>
+  <si>
+    <t>int fieldSizeSlo=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=72, field of view, in degrees, of the SLO image, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>double scanFocus=readDoubleLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>double, length=1, file oofset=76, focus depth, in diopters, of camera when Oct scan was done, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>String scanPosition=readByteString(raf,4);</t>
+  </si>
+  <si>
+    <t>byte(unicode Char), length=4, file offset=84, labels which eye was examined, "OD" or "OS"), will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>BigInteger bArray = new BigInteger( readRevByteArray(raf, 8) );</t>
+  </si>
+  <si>
+    <t>raf pointer now at 96</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=96, describes type of scan pattern used: 0 = Unknown pattern, 1 = Single line scan (one B-Scan only), 2 = Circular scan (one B-Scan only), 3 = Volume scan in ART mode, 4 = Fast volume scan, 5 = Radial scan, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>int bScanHdrSize = readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=100, number of bytes per each b-scan header;</t>
+  </si>
+  <si>
+    <t>String uID=readByteString(raf, 16);</t>
+  </si>
+  <si>
+    <t>byte (unicode Char), length=16, file offset=104, unique id of oct scan, same as serial ID of raw export name, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>String rID=readByteString(raf, 16);</t>
+  </si>
+  <si>
+    <t>byte (unicode Char), length=16, file offset=120, unique identifier of the reference OCT-scan, only for progression series, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>int pID=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=136, internal patient ID used by HEYEX, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>String patientID=readByteString(raf, 21);</t>
+  </si>
+  <si>
+    <t>byte(unicode Char), length=21, file offset=140, user-defined patient ID, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>byte[] pad=readByteArray(raf, 3);</t>
+  </si>
+  <si>
+    <t>byte, length=3, file offset=161, aligns next 4-byte boundary, not used;</t>
+  </si>
+  <si>
+    <t>Date DOB=new Date( (long)((readDoubleLittleEndian(raf)-25569</t>
+  </si>
+  <si>
+    <t>double (Microsoft DATE format), length=1, fileOffset=164, patient's date of birth, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>int vID=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, file offset=172, internal visit ID used by HEYEX, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>String visitID=readByteString(raf, 24);</t>
+  </si>
+  <si>
+    <t>byte (unicode Char), length=24, file offset=176, user-defined visit ID, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>Date examDate=new Date( (long)((readDoubleLittleEndian(raf)-25569</t>
+  </si>
+  <si>
+    <t>double (Microsocft DATE format), length=1, file offset=200, date examination occurred, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>byte[] emptyBytes=readByteArray(raf, 1840);</t>
+  </si>
+  <si>
+    <t>byte, length=1840, file offset=208, spare bytes for future use, not used;</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>java_statement</t>
+  </si>
+  <si>
+    <t>r_statement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,13 +432,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -266,7 +484,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -280,23 +498,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,435 +887,824 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="105.33203125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="4">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="4">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="F6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="4">
+        <v>24</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="F7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="4">
+        <v>32</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="F8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="4">
+        <v>40</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="F9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4">
+        <v>48</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="F10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="4">
+        <v>52</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="4">
+        <v>56</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="F12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4">
+        <v>64</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="F13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="4">
+        <v>72</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="F14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="4">
+        <v>76</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>4</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="F15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="4">
+        <v>84</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+      <c r="F16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="4">
+        <v>88</v>
+      </c>
+      <c r="J16" s="4">
+        <v>8</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+      <c r="F17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="4">
+        <v>96</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
+      <c r="F18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="4">
+        <v>100</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>16</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="F19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="4">
+        <v>104</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="30">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>16</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="F20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="4">
+        <v>120</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
+      <c r="F21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="4">
+        <v>136</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
+      <c r="F22" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="4">
+        <v>140</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+      <c r="F23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="4">
+        <v>161</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+      <c r="F24" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="4">
+        <v>164</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+      <c r="F25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="4">
+        <v>172</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+      <c r="F26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="4">
+        <v>176</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30">
+      <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="C27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
+      <c r="F27" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="4">
+        <v>200</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>1840</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="3" t="s">
         <v>65</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" s="4">
+        <v>208</v>
+      </c>
+      <c r="J28" s="4">
+        <v>1840</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1069,6 +1719,453 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28">
+        <v>1840</v>
+      </c>
+      <c r="E28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Setup section to write code for B-Scan header reading and B-Scan reading.
</commit_message>
<xml_diff>
--- a/inst/exdata/heyex_structure.xlsx
+++ b/inst/exdata/heyex_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-24640" yWindow="0" windowWidth="24600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-32540" yWindow="0" windowWidth="32500" windowHeight="17640" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
   <si>
     <t>Version</t>
   </si>
@@ -402,6 +402,156 @@
   </si>
   <si>
     <t>r_statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BScanHdrSize </t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumSeg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OffSeg </t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f </t>
+  </si>
+  <si>
+    <t>bscan_header$version &lt;- readBin(vol_file, "raw", size =1, n = 12) %&gt;% rawToChar()</t>
+  </si>
+  <si>
+    <t>bscan_header$start_x &lt;- readBin(vol_file, double())</t>
+  </si>
+  <si>
+    <t>bscan_header$b_scan_hdr_size &lt;- readBin(vol_file, integer())</t>
+  </si>
+  <si>
+    <t>bscan_header$start_y &lt;- readBin(vol_file, double())</t>
+  </si>
+  <si>
+    <t>bscan_header$end_x &lt;- readBin(vol_file, double())</t>
+  </si>
+  <si>
+    <t>bscan_header$end_y &lt;- readBin(vol_file, double())</t>
+  </si>
+  <si>
+    <t>bscan_header$num_seg &lt;- readBin(vol_file, integer())</t>
+  </si>
+  <si>
+    <t>bscan_header$off_seg &lt;- readBin(vol_file, integer())</t>
+  </si>
+  <si>
+    <t>bscan_header$quality &lt;- readBin(vol_file, double())</t>
+  </si>
+  <si>
+    <t>bscan_header$spare &lt;- readBin(vol_file, "raw", n = 196)</t>
+  </si>
+  <si>
+    <t>String bScanVersion=readByteString(raf, 12, firstBscanHdr);</t>
+  </si>
+  <si>
+    <t>byte(unicode Char), length=12, file offset=0, format of bscan header such as "HFS-BS-101", will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>int bScanHdrSize2 =readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, offset12, identical to bScanHeaderSize, not used;</t>
+  </si>
+  <si>
+    <t>float[] startX=new float[numBscans];</t>
+  </si>
+  <si>
+    <t>double (cast to float for drawBscans function), length=1, offset=16, x coordinate of SLO image corresponding to the B-Scan's start point in mm;</t>
+  </si>
+  <si>
+    <t>float[] startY=new float[numBscans];</t>
+  </si>
+  <si>
+    <t>double (cast to float for drawBscans function), length=1, offset=24, y coordinate of SLO image corresponding to the B-Scan's start point in mm;</t>
+  </si>
+  <si>
+    <t>float[] endX=new float[numBscans];</t>
+  </si>
+  <si>
+    <t>double (cast to float for drawBscans function), length=1, offset=32, x coordinate of SLO image corresponding to the B-Scan's end point in mm;</t>
+  </si>
+  <si>
+    <t>float[] endY=new float[numBscans];</t>
+  </si>
+  <si>
+    <t>double (cast to float for drawBscans function), length=1, offset=40, y coordinate of SLO image corresponding to the B-Scan's end point in mm;</t>
+  </si>
+  <si>
+    <t>int numSeg=readIntLittleEndian(raf, firstBscanHdr + 48);</t>
+  </si>
+  <si>
+    <t>integer, length=1, offset=48, number of segmentation vectors, usually two (ILM and RPE), can be 3 with NFL in circular scan mode only, here we read first bscan only and assume all bscans are equal, alternative could cehck all bscans looking for maximum;</t>
+  </si>
+  <si>
+    <t>int segOffset=readIntLittleEndian(raf);</t>
+  </si>
+  <si>
+    <t>integer, length=1, offset=52, offset to array of segmentation vectors from beginning of bscan block, here we read first bscan only and assume all bscans are equal;</t>
+  </si>
+  <si>
+    <t>float[] quality=new float[numBscans];</t>
+  </si>
+  <si>
+    <t>float, length=1, offset=56, quality of oct reflectance signal during scan, in dB, will be used in future update to provide info;</t>
+  </si>
+  <si>
+    <t>byte[] emptyBytes2=readByteArray(raf, 196);</t>
+  </si>
+  <si>
+    <t>byte, length=196, offset=60, spare bytes for future use, not used;</t>
+  </si>
+  <si>
+    <t>int segArraySize=numBscans*numSeg*sizeX;</t>
+  </si>
+  <si>
+    <t>length to make segArray;</t>
+  </si>
+  <si>
+    <t>float[] segArray=new float[segArraySize];</t>
+  </si>
+  <si>
+    <t>array of float, length=sizeX*numSeg, offset=256, y coordinates of segmentation layers (x coordinates are the sequence read from o to sizeX-1), ordered by 0 to sizeX-1 of ILM followed by 0 to sizeX-1 of RPE and, for circular scans, followed by 0 to sizeX-1 of NFL;</t>
+  </si>
+  <si>
+    <t>int segArrayByteSize=4*segArraySize;</t>
+  </si>
+  <si>
+    <t>byte length of segArray for offset purposes;</t>
+  </si>
+  <si>
+    <t>r_code</t>
+  </si>
+  <si>
+    <t>java_code</t>
+  </si>
+  <si>
+    <t>java_comments</t>
+  </si>
+  <si>
+    <t>bytes_read</t>
   </si>
 </sst>
 </file>
@@ -455,7 +605,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +624,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -484,7 +640,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -512,8 +668,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -530,8 +698,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -545,6 +728,12 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -558,6 +747,12 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -889,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+    <sheetView topLeftCell="F6" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -2167,13 +2362,335 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53" style="4" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30">
+      <c r="A2" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="8">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <f>F3-F2</f>
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G11" si="0">F4-F3</f>
+        <v>4</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="4">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="4">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30">
+      <c r="A6" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="4">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="4">
+        <v>40</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60">
+      <c r="A8" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="4">
+        <v>48</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45">
+      <c r="A9" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="4">
+        <v>52</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
+      <c r="A10" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="4">
+        <v>56</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8">
+        <v>196</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F11" s="4">
+        <v>60</v>
+      </c>
+      <c r="G11" s="4">
+        <f>F13-F11</f>
+        <v>196</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1">
+      <c r="E12" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="60">
+      <c r="E13" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="10">
+        <v>256</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="10" customFormat="1">
+      <c r="E14" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>